<commit_message>
add notes about template during covid + add to change log
</commit_message>
<xml_diff>
--- a/templates/HFR_Submission_Template_Long.xlsx
+++ b/templates/HFR_Submission_Template_Long.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achafetz\Documents\GitHub\Wavelength\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D09E44-DED0-4BE0-A55A-96560BA5E6F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12690" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="5" r:id="rId1"/>
@@ -207,7 +213,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -569,6 +575,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -590,7 +599,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -617,6 +632,100 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4381500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>7267575</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5095FA19-CF81-42AE-A1C3-D1E5ADC724AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8420100" y="152400"/>
+          <a:ext cx="2886075" cy="1362075"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:latin typeface="Gill Sans MT" panose="020B0502020104020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>During the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:latin typeface="Gill Sans MT" panose="020B0502020104020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>COVID response (2020.07 onwards), guidance has been modified to allow total numerators (no age sex) and full period reporting is acceptable for all indicators to reduce reporting burden.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:latin typeface="Gill Sans MT" panose="020B0502020104020203" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -908,7 +1017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I73"/>
   <sheetViews>
@@ -946,7 +1055,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="11">
-        <v>1.01</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -1286,7 +1395,7 @@
     <row r="72" x14ac:dyDescent="0.25"/>
     <row r="73" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection password="B386" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/mV2VMCTVIaFGzuV14lFm+84YzoZERIMVvjMAYTQpjizf/T+CsLsE5UK90Y8PNXwKQXNYzP6nuSEQLXXMkd92A==" saltValue="1MGUBJghA39laBkOa3odCQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="C2:C3">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>LEN(C2)=0</formula>
@@ -1299,7 +1408,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M1000"/>
   <sheetViews>

</xml_diff>